<commit_message>
- Add navigation wrapping issue in bug tracker
</commit_message>
<xml_diff>
--- a/Bug Tracking.xlsx
+++ b/Bug Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Work\FCC\Product Landing Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9375C2EC-400C-49A7-9E75-023E6ACA9F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FF8AB6-8DC1-4244-BE58-FAEE0916040A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{69806D31-651E-4747-818C-E533C3A7BC0D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Bug ID</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Attachments</t>
   </si>
   <si>
-    <t>Assigned To</t>
-  </si>
-  <si>
     <t>Date Reported</t>
   </si>
   <si>
@@ -80,12 +77,6 @@
     <t>Windows 10, Chrome 89</t>
   </si>
   <si>
-    <t>[link]</t>
-  </si>
-  <si>
-    <t>Jane Smith</t>
-  </si>
-  <si>
     <t>Initial report</t>
   </si>
   <si>
@@ -93,23 +84,45 @@
   </si>
   <si>
     <t>Navigation misalignment</t>
-  </si>
-  <si>
-    <t>Between width sizes 1457 to 1757px, navigation menu links will flush left instead of being centered.</t>
   </si>
   <si>
     <t>1. Navigate to home page on a desktop or large tablet
 2. Resize window to a width between 1457px to 1757px</t>
+  </si>
+  <si>
+    <t>Navigation links wrapping</t>
+  </si>
+  <si>
+    <t>Between width sizes 1457 to 1757px, navigation menu and site name links will flush left instead of being centered.</t>
+  </si>
+  <si>
+    <t>Between width sizes 1023 to 1157px, navigation menu links will wrap to a new line despite a large amount of space on either side still available</t>
+  </si>
+  <si>
+    <t>1. Navigate to home page on a desktop or large tablet
+2. Resize window to a width between 1023px to 1157px</t>
+  </si>
+  <si>
+    <t>Windows 10, Chrome 90</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -483,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E98887A-B40A-48C0-A709-1B5F0A34027D}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,12 +512,11 @@
     <col min="7" max="7" width="6.44140625" customWidth="1"/>
     <col min="8" max="8" width="21.5546875" customWidth="1"/>
     <col min="9" max="9" width="15.109375" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,49 +550,79 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="4">
+        <v>45403</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="4">
+        <v>45403</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="4">
-        <v>45403</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- Track bug where heading is cut off when using navigation   links to jump to a section
</commit_message>
<xml_diff>
--- a/Bug Tracking.xlsx
+++ b/Bug Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Work\FCC\Product Landing Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FF8AB6-8DC1-4244-BE58-FAEE0916040A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101C02BA-3614-48B6-A2DB-5F6FE1A4442B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{69806D31-651E-4747-818C-E533C3A7BC0D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Bug ID</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Open</t>
-  </si>
-  <si>
-    <t>Windows 10, Chrome 89</t>
   </si>
   <si>
     <t>Initial report</t>
@@ -103,10 +100,20 @@
 2. Resize window to a width between 1023px to 1157px</t>
   </si>
   <si>
-    <t>Windows 10, Chrome 90</t>
-  </si>
-  <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Top of section cut off on navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clicking on a navigation link will correctly jump to the right section, but the top with the heading is cut off. </t>
+  </si>
+  <si>
+    <t>1. Open menu(if on mobile)
+2. Click on a navigation link (testimonials, why adopt? Or contact)</t>
+  </si>
+  <si>
+    <t>Windows 10, Chrome</t>
   </si>
 </sst>
 </file>
@@ -496,31 +503,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E98887A-B40A-48C0-A709-1B5F0A34027D}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" customWidth="1"/>
-    <col min="7" max="7" width="6.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="21.5546875" customWidth="1"/>
     <col min="9" max="9" width="15.109375" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -529,13 +536,13 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -544,10 +551,10 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -555,70 +562,105 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J2" s="4">
         <v>45403</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J3" s="4">
         <v>45403</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="4">
+        <v>45405</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>